<commit_message>
Add sensitivity characteristics for MQ131 metal
</commit_message>
<xml_diff>
--- a/datasheet/Sensitivity_curves.xlsx
+++ b/datasheet/Sensitivity_curves.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ols/git/Arduino-MQ131-driver/datasheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4DDBD0-DCC8-5A4D-9C99-D32F46AAC576}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED2BABB-880A-CC43-B293-C237FF9FD4BD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20020" yWindow="460" windowWidth="25600" windowHeight="27000" xr2:uid="{C31139D4-38F9-5144-822A-899005BA4EB0}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27000" xr2:uid="{C31139D4-38F9-5144-822A-899005BA4EB0}"/>
   </bookViews>
   <sheets>
     <sheet name="MQ131-black" sheetId="3" r:id="rId1"/>
+    <sheet name="MQ131-metal" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>ppm</t>
   </si>
@@ -67,6 +68,9 @@
   </si>
   <si>
     <t>Temp (°C)</t>
+  </si>
+  <si>
+    <t>MQ131 (Metal)</t>
   </si>
 </sst>
 </file>
@@ -157,27 +161,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -242,6 +233,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2597,6 +2610,1596 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-CCBF-0241-BB0B-8A5ECDAFC3A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="435883135"/>
+        <c:axId val="435884383"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="435883135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435884383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="435884383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.9"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435883135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>O3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MQ131-metal'!$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ppm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.3267811403092682E-2"/>
+                  <c:y val="-9.531195528039911E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$A$38:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$B$38:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CD55-FF4F-8C41-9D1F5B20FDDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="384404207"/>
+        <c:axId val="296286383"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="384404207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296286383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="296286383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="384404207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sensitivity</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Characteristics</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MQ131-metal'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rs/R0 O3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$A$6:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$B$6:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-96AA-E742-8026-5604F2EF4F9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="435868271"/>
+        <c:axId val="435869951"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="435868271"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435869951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="435869951"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="1.0000000000000002E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435868271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Influence</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Temperature/Humidity on resistance ratio Rs/R0</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MQ131-metal'!$B$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>60% Hum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.688042226487524"/>
+                  <c:y val="-0.47768921428681066"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$A$56:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$B$56:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-34FB-E64A-9B1A-3A8CD7DAAFA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MQ131-metal'!$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30% Hum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.67268714011516317"/>
+                  <c:y val="-0.55590980951942415"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$A$56:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$C$56:$C$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-34FB-E64A-9B1A-3A8CD7DAAFA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MQ131-metal'!$D$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>85% Hum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.70723608445297503"/>
+                  <c:y val="-0.39526592070728001"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$A$56:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MQ131-metal'!$D$56:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-34FB-E64A-9B1A-3A8CD7DAAFA9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3026,6 +4629,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4971,6 +6694,1464 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5643,8 +8824,127 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94140702-A017-BF4D-A519-8F3E90B232C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{998BB64A-0044-4846-B70A-B0B1BAB9029C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{232719B5-3991-3E4A-A630-564E7757E4E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC3EBC91-A6EC-EF41-B88C-8EE6CA41C528}" name="Table1" displayName="Table1" ref="A5:D10" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC3EBC91-A6EC-EF41-B88C-8EE6CA41C528}" name="Table1" displayName="Table1" ref="A5:D10" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A5:D10" xr:uid="{187AC7DF-F74C-3449-A57E-29E6156055B3}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{54E9389B-17C2-4B4B-8046-BD403932BF48}" name="ppm"/>
@@ -5657,7 +8957,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5370191-2BA5-444A-AFC7-78BEE24C9DF8}" name="Table2" displayName="Table2" ref="A37:B42" totalsRowShown="0" headerRowDxfId="1" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E5370191-2BA5-444A-AFC7-78BEE24C9DF8}" name="Table2" displayName="Table2" ref="A37:B42" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A37:B42" xr:uid="{4EC90098-BA39-1F4E-A803-1439A56715C0}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1758A4A2-4705-724E-A6DE-1A972C938640}" name="Rs/R0 NOx" dataDxfId="7"/>
@@ -5668,7 +8968,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DEA1B590-A888-3945-8956-275AE7EF56E0}" name="Table3" displayName="Table3" ref="A56:B61" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DEA1B590-A888-3945-8956-275AE7EF56E0}" name="Table3" displayName="Table3" ref="A56:B61" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A56:B61" xr:uid="{03BE280C-4E19-5746-A006-AF7905CD1084}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CD3A47FA-7FC9-0243-BAEB-EF7653787F3D}" name="Rs/R0 CL2"/>
@@ -5679,7 +8979,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D0BAF09F-B6B5-D749-98CA-1059D0FE6D3F}" name="Table4" displayName="Table4" ref="A74:B79" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D0BAF09F-B6B5-D749-98CA-1059D0FE6D3F}" name="Table4" displayName="Table4" ref="A74:B79" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A74:B79" xr:uid="{5BA3FEEF-229E-6244-AB51-3FD355D1344E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{15ED33C0-6F64-F241-9018-F23294D8BF12}" name="Rs/R0 O3"/>
@@ -5690,13 +8990,48 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A3D6E9DD-3D66-5441-9E83-006E7A378DC8}" name="Table5" displayName="Table5" ref="A92:D100" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A3D6E9DD-3D66-5441-9E83-006E7A378DC8}" name="Table5" displayName="Table5" ref="A92:D100" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A92:D100" xr:uid="{548C53A6-F6A9-FD4E-986D-AE4C1DC18978}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C66C4C25-C90F-7248-889A-271BDEC6FBB3}" name="Temp (°C)"/>
     <tableColumn id="2" xr3:uid="{7FB1B544-147F-2F46-B10B-A629F5589787}" name="60% Hum"/>
     <tableColumn id="3" xr3:uid="{7CDB6234-8796-1F43-997F-F0735AD153E8}" name="30% Hum"/>
     <tableColumn id="4" xr3:uid="{11C08DB0-FBD0-3B47-BB6E-50898EB7A7BD}" name="85% Hum"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{239B6DEF-C938-2541-A79C-4DF65B42830B}" name="Table17" displayName="Table17" ref="A5:B11" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A5:B11" xr:uid="{187AC7DF-F74C-3449-A57E-29E6156055B3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C68BAAA8-7A9B-3549-B49D-AB45CEB9D4BF}" name="ppm"/>
+    <tableColumn id="2" xr3:uid="{C9295F06-9A06-6F45-A006-BD1B3495EA8E}" name="Rs/R0 O3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6262E926-7604-CB4C-8422-B01DC0D773F7}" name="Table410" displayName="Table410" ref="A37:B43" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A37:B43" xr:uid="{5BA3FEEF-229E-6244-AB51-3FD355D1344E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9EBF5DCB-D20E-E245-A06A-A6F256C145EC}" name="Rs/R0 O3"/>
+    <tableColumn id="2" xr3:uid="{0034E073-DF67-9D43-9BEF-1D25B7C24AD1}" name="ppm"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9C92E0EC-588B-EE45-A3CD-F738A1B67788}" name="Table511" displayName="Table511" ref="A55:D63" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A55:D63" xr:uid="{548C53A6-F6A9-FD4E-986D-AE4C1DC18978}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C0FA8CC5-5357-D648-AA0C-7E6C6E34D5FB}" name="Temp (°C)"/>
+    <tableColumn id="2" xr3:uid="{17924B17-20D6-CF43-A09F-0DF014962E31}" name="60% Hum"/>
+    <tableColumn id="3" xr3:uid="{3EEBC43A-777E-2846-9FF7-E1E05E534A6D}" name="30% Hum"/>
+    <tableColumn id="4" xr3:uid="{67D50623-E9AA-494A-92FF-BA4E93E4FB9F}" name="85% Hum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6476,4 +9811,331 @@
     <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC85215E-79D9-0644-9A7C-A59B15E431D1}">
+  <dimension ref="A1:N63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="4" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="31">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="22" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" ht="17" thickTop="1"/>
+    <row r="5" spans="1:14">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>200</v>
+      </c>
+      <c r="B9">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>500</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="22" thickBot="1">
+      <c r="A35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+    </row>
+    <row r="36" spans="1:14" ht="17" thickTop="1"/>
+    <row r="37" spans="1:14">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>1.2</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>2.7</v>
+      </c>
+      <c r="B40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B41">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="22" thickBot="1">
+      <c r="A53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+    </row>
+    <row r="54" spans="1:14" ht="17" thickTop="1"/>
+    <row r="55" spans="1:14">
+      <c r="A55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56">
+        <v>-10</v>
+      </c>
+      <c r="B56">
+        <v>1.45</v>
+      </c>
+      <c r="C56">
+        <v>1.71</v>
+      </c>
+      <c r="D56">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57">
+        <v>-5</v>
+      </c>
+      <c r="B57">
+        <v>1.38</v>
+      </c>
+      <c r="C57">
+        <v>1.62</v>
+      </c>
+      <c r="D57">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>1.34</v>
+      </c>
+      <c r="C58">
+        <v>1.58</v>
+      </c>
+      <c r="D58">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>1.21</v>
+      </c>
+      <c r="C59">
+        <v>1.42</v>
+      </c>
+      <c r="D59">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>1.06</v>
+      </c>
+      <c r="C60">
+        <v>1.26</v>
+      </c>
+      <c r="D60">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61">
+        <v>30</v>
+      </c>
+      <c r="B61">
+        <v>0.97</v>
+      </c>
+      <c r="C61">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="D61">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62">
+        <v>40</v>
+      </c>
+      <c r="B62">
+        <v>0.85</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63">
+        <v>50</v>
+      </c>
+      <c r="B63">
+        <v>0.74</v>
+      </c>
+      <c r="C63">
+        <v>0.86</v>
+      </c>
+      <c r="D63">
+        <v>0.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>